<commit_message>
Assignment-5 Arrays in progress
</commit_message>
<xml_diff>
--- a/Problems_Tracking.xlsx
+++ b/Problems_Tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecb6afe25b8f4bd1/Desktop/Java/dev-java-dsa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="225" documentId="13_ncr:1_{21BC0D0A-6F38-47BD-863E-247F45840BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89654C4D-8E63-4BB6-9C9C-3FEE2CBB2B54}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="13_ncr:1_{21BC0D0A-6F38-47BD-863E-247F45840BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E180A0F4-8E0D-4105-A69E-CBC5011B1D5F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{C572EB19-D657-424D-ADB9-C099AB151136}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="4" xr2:uid="{C572EB19-D657-424D-ADB9-C099AB151136}"/>
   </bookViews>
   <sheets>
     <sheet name="1-Flow-of-program" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="730">
   <si>
     <t>Input a year and find whether it is a leap year or not.</t>
   </si>
@@ -2239,6 +2239,9 @@
   </si>
   <si>
     <t>Not done but simple one so ignoring for now</t>
+  </si>
+  <si>
+    <t>Copy paniten sorry</t>
   </si>
 </sst>
 </file>
@@ -5465,10 +5468,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07152D1-84DE-4127-B09B-EA6B90AE33F8}">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5594,86 +5597,101 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B16" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B17" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B18" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C19" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>126</v>
       </c>

</xml_diff>